<commit_message>
ThreadManager first implementation. @TODO init thread table and set statuses.
</commit_message>
<xml_diff>
--- a/CSCI447-work-log.xlsx
+++ b/CSCI447-work-log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\harry\csci447\csci447_w21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF1E165-72DD-4026-9139-D33704758C13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD57237D-F793-4501-B8D3-04CCD81BD7D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Reading a3.pdf, adding files to GitLab, setting up spreadsheet</t>
+  </si>
+  <si>
+    <t>Threads and ThreadManager</t>
   </si>
 </sst>
 </file>
@@ -62,7 +65,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -95,7 +98,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,7 +416,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -454,15 +457,15 @@
         <v>0.75</v>
       </c>
       <c r="C2" s="3">
-        <v>0.875</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="D2" s="3">
         <f>C2-B2</f>
-        <v>0.125</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="E2" s="3">
         <f>D2</f>
-        <v>0.125</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -470,27 +473,30 @@
     </row>
     <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>44220</v>
+        <v>44221</v>
       </c>
       <c r="B3" s="3">
-        <v>0.83333333333333337</v>
+        <v>0.9159722222222223</v>
       </c>
       <c r="C3" s="3">
-        <v>0.875</v>
+        <v>0.99930555555555556</v>
       </c>
       <c r="D3" s="3">
         <f>C3-B3</f>
-        <v>4.166666666666663E-2</v>
+        <v>8.3333333333333259E-2</v>
       </c>
       <c r="E3" s="3">
         <f>D3+E2</f>
-        <v>0.16666666666666663</v>
+        <v>0.12499999999999989</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Updated work log for a5.
</commit_message>
<xml_diff>
--- a/CSCI447-work-log.xlsx
+++ b/CSCI447-work-log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\harry\csci447\csci447_w21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9525E94-7F87-4E1E-92E7-B6D96A039F69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A7F9F7-2771-4299-8DE1-C4FAE5CC83B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43410" yWindow="3300" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -45,9 +45,6 @@
     <t>End</t>
   </si>
   <si>
-    <t>Session</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -79,6 +76,30 @@
   </si>
   <si>
     <t>Exec</t>
+  </si>
+  <si>
+    <t>Adding files and reading documentaion</t>
+  </si>
+  <si>
+    <t>First implementation. Stopped after incorrectly setting pointer to user stack.</t>
+  </si>
+  <si>
+    <t>Fixed issues from a3</t>
+  </si>
+  <si>
+    <t>Fixed the user stack pointer issue, passing all fork and join tests</t>
+  </si>
+  <si>
+    <t>Correctly set errors for process by passing errors to parent.</t>
+  </si>
+  <si>
+    <t>Fixed more issues with errors</t>
+  </si>
+  <si>
+    <t>Implementeded stat</t>
+  </si>
+  <si>
+    <t>implemented command line arguments</t>
   </si>
 </sst>
 </file>
@@ -115,11 +136,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,18 +457,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="11.5703125" style="3"/>
-    <col min="4" max="4" width="12.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="4" customWidth="1"/>
     <col min="6" max="6" width="87.7109375" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
   </cols>
@@ -460,14 +484,11 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -480,16 +501,14 @@
       <c r="C2" s="3">
         <v>0.79166666666666663</v>
       </c>
-      <c r="D2" s="3">
-        <f t="shared" ref="D2:D6" si="0">C2-B2</f>
-        <v>4.166666666666663E-2</v>
-      </c>
-      <c r="E2" s="3">
-        <f>D2</f>
-        <v>4.166666666666663E-2</v>
+      <c r="D2" s="5">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E2" s="5">
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -497,21 +516,20 @@
         <v>44221</v>
       </c>
       <c r="B3" s="3">
-        <v>0.9159722222222223</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="C3" s="3">
-        <v>0.99930555555555556</v>
-      </c>
-      <c r="D3" s="3">
-        <f t="shared" si="0"/>
-        <v>8.3333333333333259E-2</v>
-      </c>
-      <c r="E3" s="3">
-        <f>D3+E2</f>
-        <v>0.12499999999999989</v>
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E3" s="5">
+        <f>SUM(E2,D3)</f>
+        <v>0.125</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -524,16 +542,15 @@
       <c r="C4" s="3">
         <v>0.64583333333333337</v>
       </c>
-      <c r="D4" s="3">
-        <f t="shared" si="0"/>
-        <v>2.083333333333337E-2</v>
-      </c>
-      <c r="E4" s="3">
-        <f>D4+E3</f>
-        <v>0.14583333333333326</v>
+      <c r="D4" s="5">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E4" s="5">
+        <f>SUM(E3,D4)</f>
+        <v>0.14583333333333334</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -546,16 +563,15 @@
       <c r="C5" s="3">
         <v>0.8125</v>
       </c>
-      <c r="D5" s="3">
-        <f t="shared" si="0"/>
-        <v>0.10416666666666663</v>
-      </c>
-      <c r="E5" s="3">
-        <f>D5+E4</f>
-        <v>0.24999999999999989</v>
+      <c r="D5" s="5">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="E5" s="5">
+        <f>SUM(E4,D5)</f>
+        <v>0.25</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -568,16 +584,15 @@
       <c r="C6" s="3">
         <v>0.91666666666666663</v>
       </c>
-      <c r="D6" s="3">
-        <f t="shared" si="0"/>
+      <c r="D6" s="5">
         <v>6.25E-2</v>
       </c>
-      <c r="E6" s="3">
-        <f>D6+E5</f>
-        <v>0.31249999999999989</v>
+      <c r="E6" s="5">
+        <f>SUM(E5,D6)</f>
+        <v>0.3125</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -585,21 +600,20 @@
         <v>44233</v>
       </c>
       <c r="B9" s="3">
-        <v>0.9159722222222223</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="C9" s="3">
-        <v>0.99930555555555556</v>
-      </c>
-      <c r="D9" s="3">
-        <f>C9-B9</f>
-        <v>8.3333333333333259E-2</v>
-      </c>
-      <c r="E9" s="3">
-        <f>D9</f>
-        <v>8.3333333333333259E-2</v>
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E9" s="5">
+        <f>SUM(E8,D9)</f>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -607,21 +621,20 @@
         <v>44234</v>
       </c>
       <c r="B10" s="3">
-        <v>0.41597222222222219</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="C10" s="3">
-        <v>0.4993055555555555</v>
-      </c>
-      <c r="D10" s="3">
-        <f>C10-B10</f>
-        <v>8.3333333333333315E-2</v>
-      </c>
-      <c r="E10" s="3">
-        <f>D10+E9</f>
-        <v>0.16666666666666657</v>
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E10" s="5">
+        <f>SUM(E9,D10)</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -632,18 +645,17 @@
         <v>0.5</v>
       </c>
       <c r="C11" s="3">
-        <v>0.99930555555555556</v>
-      </c>
-      <c r="D11" s="3">
-        <f t="shared" ref="D11:D12" si="1">C11-B11</f>
-        <v>0.49930555555555556</v>
-      </c>
-      <c r="E11" s="3">
-        <f>D11+E10</f>
-        <v>0.66597222222222219</v>
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="5">
+        <f>SUM(E10,D11)</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -656,16 +668,189 @@
       <c r="C12" s="3">
         <v>0.1875</v>
       </c>
-      <c r="D12" s="3">
-        <f t="shared" si="1"/>
+      <c r="D12" s="5">
         <v>0.1875</v>
       </c>
-      <c r="E12" s="3">
-        <f>D12+E11</f>
-        <v>0.85347222222222219</v>
+      <c r="E12" s="5">
+        <f>SUM(E11,D12)</f>
+        <v>0.85416666666666663</v>
       </c>
       <c r="F12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>44243</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D14" s="5">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" ref="E14:E22" si="0">SUM(E13,D14)</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F14" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>44243</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="0"/>
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="F15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>44251</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="0"/>
+        <v>0.8125</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>44255</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D17" s="5">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="0"/>
+        <v>0.875</v>
+      </c>
+      <c r="F17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>44258</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D18" s="5">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="0"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>44259</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0.125</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="0"/>
+        <v>1.0416666666666665</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>44261</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0</v>
+      </c>
+      <c r="D20" s="5">
+        <v>0.125</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="0"/>
+        <v>1.1666666666666665</v>
+      </c>
+      <c r="F20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>44262</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E22" s="5">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>